<commit_message>
life could be a dream
</commit_message>
<xml_diff>
--- a/Схема роботи.xlsx
+++ b/Схема роботи.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\GITRepos\-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B50CD0E-ED7A-4236-BBD6-43FE9C08F003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4C89DB-392E-41F6-A5F3-06DA2F680A78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,7 +771,7 @@
   <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,16 +918,16 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="19">
         <v>43802</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="20">
         <v>2</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="21">
         <f t="shared" si="0"/>
         <v>43804</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="29">
-        <f t="shared" ref="E19:E23" si="2">SUM(C19:D19)</f>
+        <f t="shared" ref="E19:E22" si="2">SUM(C19:D19)</f>
         <v>43813</v>
       </c>
     </row>

</xml_diff>